<commit_message>
add conflicts and availabe times show
</commit_message>
<xml_diff>
--- a/backend/media/conflicts.xlsx
+++ b/backend/media/conflicts.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="تعارضات الدكاترة" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="تعارضات الجدول" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,18 +434,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="29" customWidth="1" min="1" max="1"/>
-    <col width="78" customWidth="1" min="2" max="2"/>
+    <col width="240" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>conflicts_type</t>
+          <t>نوع التعارض</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>conflicts_detail</t>
+          <t>تفاصيل التعارض</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,319 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>اسم الدكتور: إسماعيل الصباحي , اليوم:السبت , الوقت: 12-2 الأوقات المتاحة: []</t>
+          <t>اسم الدكتور: ا. خالد الكحسه, اليوم: الخميس, الوقت: 8-10, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10, الاثنين 10-12, الاثنين 12-2, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: إيهاب الحروي, اليوم: الاثنين, الوقت: 12-2, الأوقات المتاحة: الأربعاء 10-12, الأربعاء 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: هديل دماج, اليوم: الثلاثاء, الوقت: 10-12, الأوقات المتاحة: الخميس 10-12, الخميس 12-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د نشوان المجمر, اليوم: الخميس, الوقت: 12-2, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د. فهد الاغبري, اليوم: الأربعاء, الوقت: 12-2, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10, الاثنين 10-12, الاثنين 12-2, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ا. خالد الكحسه, اليوم: السبت, الوقت: 12-2, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10, الاثنين 10-12, الاثنين 12-2, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: خولة صادق, اليوم: السبت, الوقت: 10-12, الأوقات المتاحة: الخميس 10-12, الخميس 12-2, السبت 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: عبدالقوي الفقيه, اليوم: الاثنين, الوقت: 10-12, الأوقات المتاحة: الأربعاء 10-12, الأربعاء 12-2, الأربعاء 8-10, الخميس 10-12, الخميس 12-2, الخميس 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ا. معافر منصور, اليوم: الخميس, الوقت: 12-2, الأوقات المتاحة: الأحد 10-12, الأحد 8-10, الاثنين 12-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د. ندى الحميدي, اليوم: الخميس, الوقت: 8-10, الأوقات المتاحة: الثلاثاء 10-12, الثلاثاء 12-2, الثلاثاء 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: إسماعيل الصباحي, اليوم: السبت, الوقت: 12-2, الأوقات المتاحة: الخميس 12-2, الخميس 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: عبده صالح, اليوم: الخميس, الوقت: 8-10, الأوقات المتاحة: الثلاثاء 12-2, الثلاثاء 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: خديجة الشيخ, اليوم: السبت, الوقت: 12-2, الأوقات المتاحة: الاثنين 10-12, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: علي الحمادي, اليوم: الأربعاء, الوقت: 12-2, الأوقات المتاحة: الخميس 10-12, السبت 10-12, السبت 12-2, السبت 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ا. وفاء بركات, اليوم: السبت, الوقت: 12-2, الأوقات المتاحة: الأربعاء 10-12, الأربعاء 8-10, الاثنين 10-12, الاثنين 12-2, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د. احمد مهيوب, اليوم: الأربعاء, الوقت: 8-10, الأوقات المتاحة: الاثنين 10-12, الاثنين 12-2, الاثنين 8-10, الثلاثاء 8-10, الخميس 10-12, الخميس 12-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ليلى الشعيبي, اليوم: الخميس, الوقت: 10-12, الأوقات المتاحة: الأربعاء 10-12, الأربعاء 12-2, الأربعاء 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د. محمد خشافه, اليوم: الأربعاء, الوقت: 10-12, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الاثنين 10-12, الاثنين 12-2, الاثنين 8-10, الثلاثاء 10-12, الثلاثاء 12-2, الثلاثاء 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د. ناجي غلاب, اليوم: الأربعاء, الوقت: 12-2, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10, الاثنين 10-12, الاثنين 12-2, الاثنين 8-10, الثلاثاء 10-12, الثلاثاء 12-2, الثلاثاء 8-10, الخميس 10-12, الخميس 12-2, الخميس 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: محمد الطيب, اليوم: الخميس, الوقت: 10-12, الأوقات المتاحة: الأربعاء 8-10, الثلاثاء 12-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ا. وفاء بركات, اليوم: الأحد, الوقت: 10-12, الأوقات المتاحة: الأربعاء 10-12, الأربعاء 8-10, الاثنين 10-12, الاثنين 12-2, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: لينا الفقية, اليوم: الاثنين, الوقت: 12-2, الأوقات المتاحة: الاثنين 10-12, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د. عبدالباسط الادريسي, اليوم: الثلاثاء, الوقت: 10-12, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الاثنين 10-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ا. فؤاد الهمداني, اليوم: الخميس, الوقت: 12-2, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ا.هناء العبيدي, اليوم: الخميس, الوقت: 10-12, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: د. عادل العفيري, اليوم: الثلاثاء, الوقت: 12-2, الأوقات المتاحة: الاثنين 10-12, الاثنين 12-2, الاثنين 8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>تم تعيين دكتور في غير موعدة</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>اسم الدكتور: ا. صلاح امين, اليوم: الخميس, الوقت: 10-12, الأوقات المتاحة: الأحد 10-12, الأحد 12-2, الأحد 8-10, الاثنين 10-12, الاثنين 8-10</t>
         </is>
       </c>
     </row>

</xml_diff>